<commit_message>
update read me ^ redirect report
</commit_message>
<xml_diff>
--- a/datatest/RegisterMiniAppPlan.xlsx
+++ b/datatest/RegisterMiniAppPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngan.dang/Testing/mini-app-center/datatest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA5D691-24C5-134A-8947-E06006ED8A9E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53823B70-8FAC-2944-A403-867F5CD44AED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="5520" windowWidth="22280" windowHeight="11320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8060" yWindow="8440" windowWidth="22280" windowHeight="11320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterMiniAppPlan" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
     <t>App team accept</t>
   </si>
   <si>
-    <t>Bear Coffee 23</t>
+    <t>Bear Coffee 30</t>
   </si>
 </sst>
 </file>

</xml_diff>